<commit_message>
Auto-committed on 2021/12/21 週二
Former-commit-id: 01c0f3f0c62848dc90cff5f5f5820e2f61442bd1
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/XX-系統/TxControl.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/XX-系統/TxControl.xlsx
@@ -175,74 +175,76 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>修改者櫃員編號</t>
+  </si>
+  <si>
+    <t>修改日期時間</t>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>TxControl</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>作業流程控制檔</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>控制項目</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>50</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>控制內容</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>50</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Desc</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreateDate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LastUpdate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>LastUpdateEmpNo</t>
-  </si>
-  <si>
-    <t>修改者櫃員編號</t>
-  </si>
-  <si>
-    <t>LastUpdate</t>
-  </si>
-  <si>
-    <t>修改日期時間</t>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>TxControl</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>作業流程控制檔</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>控制項目</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>50</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>控制內容</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>50</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Code</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Desc</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Code</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CreateDate</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -829,7 +831,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -850,10 +852,10 @@
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="9"/>
@@ -878,7 +880,7 @@
       </c>
       <c r="B3" s="35"/>
       <c r="C3" s="28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>19</v>
@@ -956,45 +958,45 @@
     </row>
     <row r="9" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>21</v>
@@ -1011,10 +1013,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>24</v>
@@ -1028,13 +1030,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B13" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>23</v>
@@ -1045,13 +1047,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>25</v>

</xml_diff>